<commit_message>
android to android pending
</commit_message>
<xml_diff>
--- a/Test List.xlsx
+++ b/Test List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armaan/Developer/Cross-Platform-Media-Sharing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45068662-5E1F-6744-8C72-0AF809B3489D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D33A63-650B-6348-92A0-C7698A497FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="19500" xr2:uid="{A8552854-C653-244D-8B19-23593DF13A92}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FEBBFA-2179-E040-B0DF-2B80AAFE4EA3}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="193" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,7 +703,7 @@
         <v>18</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -825,13 +825,13 @@
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -916,7 +916,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>6</v>
@@ -980,7 +980,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>6</v>
@@ -1044,7 +1044,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>6</v>
@@ -1102,13 +1102,13 @@
         <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>6</v>
@@ -1208,7 +1208,7 @@
         <v>18</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>6</v>
@@ -1272,7 +1272,7 @@
         <v>18</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>6</v>
@@ -1336,7 +1336,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>6</v>
@@ -1394,13 +1394,13 @@
         <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>6</v>
@@ -1500,7 +1500,7 @@
         <v>18</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>6</v>
@@ -1564,7 +1564,7 @@
         <v>18</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>6</v>
@@ -1628,7 +1628,7 @@
         <v>18</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>6</v>
@@ -1686,13 +1686,13 @@
         <v>17</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>6</v>
@@ -1712,12 +1712,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="I37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="B26:E26"/>
     <mergeCell ref="I13:M13"/>
     <mergeCell ref="J14:M14"/>
     <mergeCell ref="I25:M25"/>
@@ -1728,6 +1722,12 @@
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="I37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="B26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
android to android issue
</commit_message>
<xml_diff>
--- a/Test List.xlsx
+++ b/Test List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armaan/Developer/Cross-Platform-Media-Sharing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D33A63-650B-6348-92A0-C7698A497FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9904A9-9C63-1B4D-A283-48FC6C9B6D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="19500" xr2:uid="{A8552854-C653-244D-8B19-23593DF13A92}"/>
   </bookViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FEBBFA-2179-E040-B0DF-2B80AAFE4EA3}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="193" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="193" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,7 +807,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -822,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>18</v>
@@ -1099,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1391,7 +1391,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>

</xml_diff>